<commit_message>
Terminado de corregir 2
</commit_message>
<xml_diff>
--- a/ejercicio2_normalizacion.xlsx
+++ b/ejercicio2_normalizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricardo.morenoventas\Desktop\SQL\SQL_04052023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22984B68-CA2A-4737-98C8-404A80AE86D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD2C8A2-67FF-451C-9478-19D0FC46FDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{3FCA0B04-F99C-4B1D-911E-0273235ADDA9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="43">
   <si>
     <t>DNI</t>
   </si>
@@ -1506,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F23BDA-5A8B-4956-8681-B3A7260AAB3B}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1586,12 +1586,9 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="10"/>
@@ -1603,13 +1600,10 @@
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1">
-        <v>125</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="C10" s="4">
         <v>36972</v>
       </c>
-      <c r="E10" s="5">
+      <c r="D10" s="5">
         <v>15000000</v>
       </c>
       <c r="F10" s="10"/>
@@ -1621,13 +1615,10 @@
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1">
-        <v>90</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11" s="4">
         <v>37025</v>
       </c>
-      <c r="E11" s="5">
+      <c r="D11" s="5">
         <v>6000000</v>
       </c>
       <c r="F11" s="10"/>
@@ -1639,13 +1630,10 @@
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1">
-        <v>125</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12" s="4">
         <v>36845</v>
       </c>
-      <c r="E12" s="5">
+      <c r="D12" s="5">
         <v>14000000</v>
       </c>
       <c r="F12" s="10"/>
@@ -1657,13 +1645,10 @@
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1">
-        <v>65</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" s="4">
         <v>34856</v>
       </c>
-      <c r="E13" s="5">
+      <c r="D13" s="5">
         <v>2500000</v>
       </c>
       <c r="F13" s="10"/>
@@ -1675,13 +1660,10 @@
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1">
-        <v>50</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="4">
         <v>32408</v>
       </c>
-      <c r="E14" s="5">
+      <c r="D14" s="5">
         <v>1800000</v>
       </c>
       <c r="F14" s="10"/>
@@ -1693,13 +1675,10 @@
       <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="1">
-        <v>50</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="C15" s="4">
         <v>32408</v>
       </c>
-      <c r="E15" s="5">
+      <c r="D15" s="5">
         <v>1800000</v>
       </c>
     </row>
@@ -1871,7 +1850,64 @@
         <v>32</v>
       </c>
     </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="1">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>